<commit_message>
Remove of possibility to import a csv file. All the files imported must now be in xlsx format.\nFormatting the date displayed by the notebook.\nA message promps now when the user clicks on the buttons update or import to tell if the action happened or failed.
</commit_message>
<xml_diff>
--- a/app/code/data/raw_copy_expenses.xlsx
+++ b/app/code/data/raw_copy_expenses.xlsx
@@ -500,29 +500,13 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="n">
-        <v>246.55</v>
-      </c>
-      <c r="C2" t="n">
-        <v>3</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Campus Laval  : 1er loyer du CAMPUS LAVAL</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2019-08-01T00:00:00</t>
-        </is>
-      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>housing:rent</t>
-        </is>
-      </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
@@ -532,25 +516,13 @@
       <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" t="n">
-        <v>545.23</v>
-      </c>
-      <c r="C3" t="n">
-        <v>3</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Avion : billet France -&gt; Québec</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>transport:plane</t>
-        </is>
-      </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
@@ -560,27 +532,13 @@
       <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="n">
-        <v>30</v>
-      </c>
+      <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Equipement fnac, oreiller</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>2019-08-04T00:00:00</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>equipement:other</t>
-        </is>
-      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
@@ -590,29 +548,13 @@
       <c r="A5" t="n">
         <v>4</v>
       </c>
-      <c r="B5" t="n">
-        <v>135</v>
-      </c>
-      <c r="C5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Pharmacie crème visage + dermatologue</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>2019-08-06T00:00:00</t>
-        </is>
-      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>health</t>
-        </is>
-      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
@@ -622,29 +564,13 @@
       <c r="A6" t="n">
         <v>5</v>
       </c>
-      <c r="B6" t="n">
-        <v>16</v>
-      </c>
-      <c r="C6" t="n">
-        <v>3</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Mcdo</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>2019-08-10T00:00:00</t>
-        </is>
-      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>alimentary</t>
-        </is>
-      </c>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
@@ -654,25 +580,13 @@
       <c r="A7" t="n">
         <v>6</v>
       </c>
-      <c r="B7" t="n">
-        <v>50</v>
-      </c>
-      <c r="C7" t="n">
-        <v>3</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Leclerc</t>
-        </is>
-      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>alimentary</t>
-        </is>
-      </c>
+      <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
@@ -682,27 +596,13 @@
       <c r="A8" t="n">
         <v>7</v>
       </c>
-      <c r="B8" t="n">
-        <v>30</v>
-      </c>
+      <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Franprix</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>2019-08-15T00:00:00</t>
-        </is>
-      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>alimentary</t>
-        </is>
-      </c>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
@@ -712,29 +612,13 @@
       <c r="A9" t="n">
         <v>8</v>
       </c>
-      <c r="B9" t="n">
-        <v>10</v>
-      </c>
+      <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Casino</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>2019-08-17T00:00:00</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>1062.78</v>
-      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>alimentary</t>
-        </is>
-      </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
@@ -755,7 +639,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2019-08-22T00:00:00</t>
+          <t>2019-08-17</t>
         </is>
       </c>
       <c r="F10" t="inlineStr"/>
@@ -893,7 +777,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2019-08-23T00:00:00</t>
+          <t>2019-08-23</t>
         </is>
       </c>
       <c r="F15" t="inlineStr"/>
@@ -1159,7 +1043,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2019-08-24T00:00:00</t>
+          <t>2019-08-24</t>
         </is>
       </c>
       <c r="F25" t="inlineStr"/>
@@ -1347,7 +1231,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2019-08-25T00:00:00</t>
+          <t>2019-08-25</t>
         </is>
       </c>
       <c r="F32" t="inlineStr"/>
@@ -1405,7 +1289,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2019-08-26T00:00:00</t>
+          <t>2019-08-26</t>
         </is>
       </c>
       <c r="F34" t="inlineStr"/>
@@ -1543,7 +1427,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2019-08-27T00:00:00</t>
+          <t>2019-08-27</t>
         </is>
       </c>
       <c r="F39" t="inlineStr"/>
@@ -1657,7 +1541,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2019-08-28T00:00:00</t>
+          <t>2019-08-28</t>
         </is>
       </c>
       <c r="F43" t="inlineStr"/>
@@ -1771,7 +1655,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2019-08-29T00:00:00</t>
+          <t>2019-08-29</t>
         </is>
       </c>
       <c r="F47" t="inlineStr"/>
@@ -1937,7 +1821,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>2019-08-30T00:00:00</t>
+          <t>2019-08-30</t>
         </is>
       </c>
       <c r="F54" t="inlineStr"/>
@@ -2031,7 +1915,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2019-08-31T00:00:00</t>
+          <t>2019-08-31</t>
         </is>
       </c>
       <c r="F58" t="inlineStr"/>
@@ -2101,7 +1985,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>2019-09-03T00:00:00</t>
+          <t>2019-09-03</t>
         </is>
       </c>
       <c r="F61" t="inlineStr"/>
@@ -2175,7 +2059,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>2019-09-05T00:00:00</t>
+          <t>2019-09-05</t>
         </is>
       </c>
       <c r="F64" t="inlineStr"/>
@@ -2223,7 +2107,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>2019-09-06T00:00:00</t>
+          <t>2019-09-06</t>
         </is>
       </c>
       <c r="F66" t="inlineStr"/>
@@ -2347,7 +2231,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>2019-09-07T00:00:00</t>
+          <t>2019-09-07</t>
         </is>
       </c>
       <c r="F71" t="inlineStr"/>
@@ -2395,7 +2279,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>2019-09-08T00:00:00</t>
+          <t>2019-09-08</t>
         </is>
       </c>
       <c r="F73" t="inlineStr"/>
@@ -2471,7 +2355,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>2019-09-09T00:00:00</t>
+          <t>2019-09-09</t>
         </is>
       </c>
       <c r="F76" t="inlineStr"/>
@@ -2563,7 +2447,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>2019-09-11T00:00:00</t>
+          <t>2019-09-11</t>
         </is>
       </c>
       <c r="F80" t="inlineStr"/>
@@ -2673,7 +2557,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>2019-09-12T00:00:00</t>
+          <t>2019-09-12</t>
         </is>
       </c>
       <c r="F85" t="inlineStr"/>
@@ -2717,7 +2601,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>2019-09-13T00:00:00</t>
+          <t>2019-09-13</t>
         </is>
       </c>
       <c r="F87" t="inlineStr"/>
@@ -2927,7 +2811,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>2019-09-15T00:00:00</t>
+          <t>2019-09-15</t>
         </is>
       </c>
       <c r="F95" t="inlineStr"/>
@@ -3001,7 +2885,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>2019-09-17T00:00:00</t>
+          <t>2019-09-17</t>
         </is>
       </c>
       <c r="F98" t="inlineStr"/>
@@ -3075,7 +2959,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>2019-09-18T00:00:00</t>
+          <t>2019-09-18</t>
         </is>
       </c>
       <c r="F101" t="inlineStr"/>
@@ -3123,7 +3007,7 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>2019-09-19T00:00:00</t>
+          <t>2019-09-19</t>
         </is>
       </c>
       <c r="F103" t="inlineStr"/>
@@ -3173,7 +3057,7 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>2019-09-20T00:00:00</t>
+          <t>2019-09-20</t>
         </is>
       </c>
       <c r="F105" t="inlineStr"/>
@@ -3325,7 +3209,7 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>2019-09-21T00:00:00</t>
+          <t>2019-09-21</t>
         </is>
       </c>
       <c r="F111" t="inlineStr"/>
@@ -3399,7 +3283,7 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>2019-09-23T00:00:00</t>
+          <t>2019-09-23</t>
         </is>
       </c>
       <c r="F114" t="inlineStr"/>
@@ -3553,7 +3437,7 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>2019-09-25T00:00:00</t>
+          <t>2019-09-25</t>
         </is>
       </c>
       <c r="F120" t="inlineStr"/>
@@ -3679,7 +3563,7 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>2019-09-26T00:00:00</t>
+          <t>2019-09-26</t>
         </is>
       </c>
       <c r="F125" t="inlineStr"/>
@@ -3833,7 +3717,7 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>2019-09-27T00:00:00</t>
+          <t>2019-09-27</t>
         </is>
       </c>
       <c r="F131" t="inlineStr"/>
@@ -3883,7 +3767,7 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>2019-09-29T00:00:00</t>
+          <t>2019-09-29</t>
         </is>
       </c>
       <c r="F133" t="inlineStr"/>
@@ -3931,7 +3815,7 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>2019-09-30T00:00:00</t>
+          <t>2019-09-30</t>
         </is>
       </c>
       <c r="F135" t="inlineStr"/>
@@ -4029,7 +3913,7 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>2019-10-03T00:00:00</t>
+          <t>2019-10-03</t>
         </is>
       </c>
       <c r="F139" t="inlineStr"/>
@@ -4105,7 +3989,7 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>2019-10-04T00:00:00</t>
+          <t>2019-10-04</t>
         </is>
       </c>
       <c r="F142" t="inlineStr"/>
@@ -4179,7 +4063,7 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>2019-10-05T00:00:00</t>
+          <t>2019-10-05</t>
         </is>
       </c>
       <c r="F145" t="inlineStr"/>
@@ -4253,7 +4137,7 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>2019-10-09T00:00:00</t>
+          <t>2019-10-09</t>
         </is>
       </c>
       <c r="F148" t="inlineStr"/>
@@ -4303,7 +4187,7 @@
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>2019-10-10T00:00:00</t>
+          <t>2019-10-10</t>
         </is>
       </c>
       <c r="F150" t="inlineStr"/>
@@ -4439,7 +4323,7 @@
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>2019-10-11T00:00:00</t>
+          <t>2019-10-11</t>
         </is>
       </c>
       <c r="F155" t="inlineStr"/>
@@ -4569,7 +4453,7 @@
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>2019-10-12T00:00:00</t>
+          <t>2019-10-12</t>
         </is>
       </c>
       <c r="F160" t="inlineStr"/>
@@ -4617,7 +4501,7 @@
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>2019-10-13T00:00:00</t>
+          <t>2019-10-13</t>
         </is>
       </c>
       <c r="F162" t="inlineStr"/>
@@ -4667,7 +4551,7 @@
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>2019-10-14T00:00:00</t>
+          <t>2019-10-14</t>
         </is>
       </c>
       <c r="F164" t="inlineStr"/>
@@ -4749,7 +4633,7 @@
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>2019-10-16T00:00:00</t>
+          <t>2019-10-16</t>
         </is>
       </c>
       <c r="F167" t="inlineStr"/>
@@ -4825,7 +4709,7 @@
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>2019-10-18T00:00:00</t>
+          <t>2019-10-18</t>
         </is>
       </c>
       <c r="F170" t="inlineStr"/>
@@ -4969,7 +4853,7 @@
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>2019-10-19T00:00:00</t>
+          <t>2019-10-19</t>
         </is>
       </c>
       <c r="F175" t="inlineStr"/>
@@ -5145,7 +5029,7 @@
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>2019-10-20T00:00:00</t>
+          <t>2019-10-20</t>
         </is>
       </c>
       <c r="F181" t="inlineStr"/>
@@ -5261,7 +5145,7 @@
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>2019-10-21T00:00:00</t>
+          <t>2019-10-21</t>
         </is>
       </c>
       <c r="F185" t="inlineStr"/>
@@ -5339,7 +5223,7 @@
       <c r="D188" t="inlineStr"/>
       <c r="E188" t="inlineStr">
         <is>
-          <t>2019-10-22T00:00:00</t>
+          <t>2019-10-22</t>
         </is>
       </c>
       <c r="F188" t="inlineStr"/>
@@ -5409,7 +5293,7 @@
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>2019-10-23T00:00:00</t>
+          <t>2019-10-23</t>
         </is>
       </c>
       <c r="F191" t="inlineStr"/>
@@ -5483,7 +5367,7 @@
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>2019-10-25T00:00:00</t>
+          <t>2019-10-25</t>
         </is>
       </c>
       <c r="F194" t="inlineStr"/>
@@ -5573,7 +5457,7 @@
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>2019-10-27T00:00:00</t>
+          <t>2019-10-27</t>
         </is>
       </c>
       <c r="F198" t="inlineStr"/>
@@ -5619,7 +5503,7 @@
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>2019-10-28T00:00:00</t>
+          <t>2019-10-28</t>
         </is>
       </c>
       <c r="F200" t="inlineStr"/>
@@ -5679,7 +5563,7 @@
       <c r="D203" t="inlineStr"/>
       <c r="E203" t="inlineStr">
         <is>
-          <t>2019-10-29T00:00:00</t>
+          <t>2019-10-29</t>
         </is>
       </c>
       <c r="F203" t="inlineStr"/>
@@ -5721,7 +5605,7 @@
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>2019-10-30T00:00:00</t>
+          <t>2019-10-30</t>
         </is>
       </c>
       <c r="F205" t="inlineStr"/>
@@ -5771,7 +5655,7 @@
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>2019-10-31T00:00:00</t>
+          <t>2019-10-31</t>
         </is>
       </c>
       <c r="F207" t="inlineStr"/>
@@ -5821,7 +5705,7 @@
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>2019-11-01T00:00:00</t>
+          <t>2019-11-01</t>
         </is>
       </c>
       <c r="F209" t="inlineStr"/>
@@ -5873,7 +5757,7 @@
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>2019-11-04T00:00:00</t>
+          <t>2019-11-04</t>
         </is>
       </c>
       <c r="F211" t="inlineStr"/>
@@ -5927,7 +5811,7 @@
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>2019-11-05T00:00:00</t>
+          <t>2019-11-05</t>
         </is>
       </c>
       <c r="F213" t="inlineStr"/>
@@ -6001,7 +5885,7 @@
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>2019-11-06T00:00:00</t>
+          <t>2019-11-06</t>
         </is>
       </c>
       <c r="F216" t="inlineStr"/>
@@ -6077,7 +5961,7 @@
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>2019-11-08T00:00:00</t>
+          <t>2019-11-08</t>
         </is>
       </c>
       <c r="F219" t="inlineStr"/>
@@ -6127,7 +6011,7 @@
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>2019-11-09T00:00:00</t>
+          <t>2019-11-09</t>
         </is>
       </c>
       <c r="F221" t="inlineStr"/>
@@ -6175,7 +6059,7 @@
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>2019-11-15T00:00:00</t>
+          <t>2019-11-15</t>
         </is>
       </c>
       <c r="F223" t="inlineStr"/>
@@ -6305,7 +6189,7 @@
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>2019-11-16T00:00:00</t>
+          <t>2019-11-16</t>
         </is>
       </c>
       <c r="F228" t="inlineStr"/>
@@ -6379,7 +6263,7 @@
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>2019-11-17T00:00:00</t>
+          <t>2019-11-17</t>
         </is>
       </c>
       <c r="F231" t="inlineStr"/>
@@ -6481,7 +6365,7 @@
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>2019-11-22T00:00:00</t>
+          <t>2019-11-22</t>
         </is>
       </c>
       <c r="F235" t="inlineStr"/>
@@ -6623,7 +6507,7 @@
       </c>
       <c r="E240" t="inlineStr">
         <is>
-          <t>2019-11-28T00:00:00</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="F240" t="inlineStr"/>
@@ -6787,7 +6671,7 @@
       </c>
       <c r="E246" t="inlineStr">
         <is>
-          <t>2019-11-29T00:00:00</t>
+          <t>2019-11-29</t>
         </is>
       </c>
       <c r="F246" t="inlineStr"/>
@@ -6881,7 +6765,7 @@
       </c>
       <c r="E250" t="inlineStr">
         <is>
-          <t>2019-12-01T00:00:00</t>
+          <t>2019-12-01</t>
         </is>
       </c>
       <c r="F250" t="inlineStr"/>
@@ -6931,7 +6815,7 @@
       </c>
       <c r="E252" t="inlineStr">
         <is>
-          <t>2019-12-03T00:00:00</t>
+          <t>2019-12-03</t>
         </is>
       </c>
       <c r="F252" t="inlineStr"/>
@@ -7007,7 +6891,7 @@
       </c>
       <c r="E255" t="inlineStr">
         <is>
-          <t>2019-12-05T00:00:00</t>
+          <t>2019-12-05</t>
         </is>
       </c>
       <c r="F255" t="inlineStr"/>
@@ -7107,7 +6991,7 @@
       </c>
       <c r="E259" t="inlineStr">
         <is>
-          <t>2019-12-09T00:00:00</t>
+          <t>2019-12-09</t>
         </is>
       </c>
       <c r="F259" t="inlineStr"/>
@@ -7155,7 +7039,7 @@
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>2019-12-10T00:00:00</t>
+          <t>2019-12-10</t>
         </is>
       </c>
       <c r="F261" t="inlineStr"/>
@@ -7203,7 +7087,7 @@
       </c>
       <c r="E263" t="inlineStr">
         <is>
-          <t>2019-12-12T00:00:00</t>
+          <t>2019-12-12</t>
         </is>
       </c>
       <c r="F263" t="inlineStr"/>
@@ -7305,7 +7189,7 @@
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>2019-12-15T00:00:00</t>
+          <t>2019-12-15</t>
         </is>
       </c>
       <c r="F267" t="inlineStr"/>
@@ -7381,7 +7265,7 @@
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>2019-12-16T00:00:00</t>
+          <t>2019-12-16</t>
         </is>
       </c>
       <c r="F270" t="inlineStr"/>
@@ -7509,7 +7393,7 @@
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>2019-12-17T00:00:00</t>
+          <t>2019-12-17</t>
         </is>
       </c>
       <c r="F275" t="inlineStr"/>
@@ -7559,7 +7443,7 @@
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>2019-12-18T00:00:00</t>
+          <t>2019-12-18</t>
         </is>
       </c>
       <c r="F277" t="inlineStr"/>
@@ -7609,7 +7493,7 @@
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>2019-12-19T00:00:00</t>
+          <t>2019-12-19</t>
         </is>
       </c>
       <c r="F279" t="inlineStr"/>
@@ -7711,7 +7595,7 @@
       </c>
       <c r="E283" t="inlineStr">
         <is>
-          <t>2019-12-22T00:00:00</t>
+          <t>2019-12-22</t>
         </is>
       </c>
       <c r="F283" t="inlineStr"/>
@@ -7869,7 +7753,7 @@
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>2019-12-25T00:00:00</t>
+          <t>2019-12-25</t>
         </is>
       </c>
       <c r="F289" t="inlineStr"/>
@@ -7971,7 +7855,7 @@
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>2019-12-26T00:00:00</t>
+          <t>2019-12-26</t>
         </is>
       </c>
       <c r="F293" t="inlineStr"/>
@@ -8099,7 +7983,7 @@
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>2019-12-31T00:00:00</t>
+          <t>2019-12-31</t>
         </is>
       </c>
       <c r="F298" t="inlineStr"/>
@@ -8175,7 +8059,7 @@
       </c>
       <c r="E301" t="inlineStr">
         <is>
-          <t>2020-01-01T00:00:00</t>
+          <t>2020-01-01</t>
         </is>
       </c>
       <c r="F301" t="inlineStr"/>
@@ -8225,7 +8109,7 @@
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t>2020-01-05T00:00:00</t>
+          <t>2020-01-05</t>
         </is>
       </c>
       <c r="F303" t="inlineStr"/>
@@ -8275,7 +8159,7 @@
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>2020-01-08T00:00:00</t>
+          <t>2020-01-08</t>
         </is>
       </c>
       <c r="F305" t="inlineStr"/>
@@ -8325,7 +8209,7 @@
       </c>
       <c r="E307" t="inlineStr">
         <is>
-          <t>2020-01-09T00:00:00</t>
+          <t>2020-01-09</t>
         </is>
       </c>
       <c r="F307" t="inlineStr"/>
@@ -8401,7 +8285,7 @@
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>2020-01-10T00:00:00</t>
+          <t>2020-01-10</t>
         </is>
       </c>
       <c r="F310" t="inlineStr"/>
@@ -8451,7 +8335,7 @@
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>2020-01-11T00:00:00</t>
+          <t>2020-01-11</t>
         </is>
       </c>
       <c r="F312" t="inlineStr"/>
@@ -8505,7 +8389,7 @@
       </c>
       <c r="E314" t="inlineStr">
         <is>
-          <t>2020-01-14T00:00:00</t>
+          <t>2020-01-14</t>
         </is>
       </c>
       <c r="F314" t="inlineStr"/>
@@ -8555,7 +8439,7 @@
       </c>
       <c r="E316" t="inlineStr">
         <is>
-          <t>2020-01-15T00:00:00</t>
+          <t>2020-01-15</t>
         </is>
       </c>
       <c r="F316" t="inlineStr"/>
@@ -8635,7 +8519,7 @@
       </c>
       <c r="E319" t="inlineStr">
         <is>
-          <t>2020-01-16T00:00:00</t>
+          <t>2020-01-16</t>
         </is>
       </c>
       <c r="F319" t="inlineStr"/>
@@ -8715,7 +8599,7 @@
       </c>
       <c r="E322" t="inlineStr">
         <is>
-          <t>2020-01-18T00:00:00</t>
+          <t>2020-01-18</t>
         </is>
       </c>
       <c r="F322" t="inlineStr"/>
@@ -8765,7 +8649,7 @@
       </c>
       <c r="E324" t="inlineStr">
         <is>
-          <t>2020-01-20T00:00:00</t>
+          <t>2020-01-20</t>
         </is>
       </c>
       <c r="F324" t="inlineStr"/>
@@ -8841,7 +8725,7 @@
       </c>
       <c r="E327" t="inlineStr">
         <is>
-          <t>2020-01-25T00:00:00</t>
+          <t>2020-01-25</t>
         </is>
       </c>
       <c r="F327" t="inlineStr"/>
@@ -8917,7 +8801,7 @@
       </c>
       <c r="E330" t="inlineStr">
         <is>
-          <t>2020-01-26T00:00:00</t>
+          <t>2020-01-26</t>
         </is>
       </c>
       <c r="F330" t="inlineStr"/>
@@ -9019,7 +8903,7 @@
       </c>
       <c r="E334" t="inlineStr">
         <is>
-          <t>2020-01-29T00:00:00</t>
+          <t>2020-01-29</t>
         </is>
       </c>
       <c r="F334" t="inlineStr"/>
@@ -9069,7 +8953,7 @@
       </c>
       <c r="E336" t="inlineStr">
         <is>
-          <t>2020-01-30T00:00:00</t>
+          <t>2020-01-30</t>
         </is>
       </c>
       <c r="F336" t="inlineStr"/>
@@ -9145,7 +9029,7 @@
       </c>
       <c r="E339" t="inlineStr">
         <is>
-          <t>2020-02-02T00:00:00</t>
+          <t>2020-02-02</t>
         </is>
       </c>
       <c r="F339" t="inlineStr"/>
@@ -9213,7 +9097,7 @@
       </c>
       <c r="E342" t="inlineStr">
         <is>
-          <t>2020-02-03T00:00:00</t>
+          <t>2020-02-03</t>
         </is>
       </c>
       <c r="F342" t="inlineStr"/>
@@ -9259,7 +9143,7 @@
       </c>
       <c r="E344" t="inlineStr">
         <is>
-          <t>2020-02-04T00:00:00</t>
+          <t>2020-02-04</t>
         </is>
       </c>
       <c r="F344" t="inlineStr"/>
@@ -9305,7 +9189,7 @@
       </c>
       <c r="E346" t="inlineStr">
         <is>
-          <t>2020-02-05T00:00:00</t>
+          <t>2020-02-05</t>
         </is>
       </c>
       <c r="F346" t="inlineStr"/>
@@ -9355,7 +9239,7 @@
       </c>
       <c r="E348" t="inlineStr">
         <is>
-          <t>2020-02-06T00:00:00</t>
+          <t>2020-02-06</t>
         </is>
       </c>
       <c r="F348" t="inlineStr"/>
@@ -9469,7 +9353,7 @@
       </c>
       <c r="E352" t="inlineStr">
         <is>
-          <t>2020-02-07T00:00:00</t>
+          <t>2020-02-07</t>
         </is>
       </c>
       <c r="F352" t="inlineStr"/>
@@ -9553,7 +9437,7 @@
       </c>
       <c r="E355" t="inlineStr">
         <is>
-          <t>2020-02-08T00:00:00</t>
+          <t>2020-02-08</t>
         </is>
       </c>
       <c r="F355" t="inlineStr"/>
@@ -9607,7 +9491,7 @@
       </c>
       <c r="E357" t="inlineStr">
         <is>
-          <t>2020-02-09T00:00:00</t>
+          <t>2020-02-09</t>
         </is>
       </c>
       <c r="F357" t="inlineStr"/>
@@ -9691,7 +9575,7 @@
       </c>
       <c r="E360" t="inlineStr">
         <is>
-          <t>2020-02-10T00:00:00</t>
+          <t>2020-02-10</t>
         </is>
       </c>
       <c r="F360" t="inlineStr"/>
@@ -9745,7 +9629,7 @@
       </c>
       <c r="E362" t="inlineStr">
         <is>
-          <t>2020-02-12T00:00:00</t>
+          <t>2020-02-12</t>
         </is>
       </c>
       <c r="F362" t="inlineStr"/>
@@ -9795,7 +9679,7 @@
       </c>
       <c r="E364" t="inlineStr">
         <is>
-          <t>2020-02-13T00:00:00</t>
+          <t>2020-02-13</t>
         </is>
       </c>
       <c r="F364" t="inlineStr"/>
@@ -9845,7 +9729,7 @@
       </c>
       <c r="E366" t="inlineStr">
         <is>
-          <t>2020-02-14T00:00:00</t>
+          <t>2020-02-14</t>
         </is>
       </c>
       <c r="F366" t="inlineStr"/>
@@ -9895,7 +9779,7 @@
       </c>
       <c r="E368" t="inlineStr">
         <is>
-          <t>2020-02-15T00:00:00</t>
+          <t>2020-02-15</t>
         </is>
       </c>
       <c r="F368" t="inlineStr"/>
@@ -9971,7 +9855,7 @@
       </c>
       <c r="E371" t="inlineStr">
         <is>
-          <t>2020-02-17T00:00:00</t>
+          <t>2020-02-17</t>
         </is>
       </c>
       <c r="F371" t="inlineStr"/>
@@ -10021,7 +9905,7 @@
       </c>
       <c r="E373" t="inlineStr">
         <is>
-          <t>2020-02-19T00:00:00</t>
+          <t>2020-02-19</t>
         </is>
       </c>
       <c r="F373" t="inlineStr"/>
@@ -10071,7 +9955,7 @@
       </c>
       <c r="E375" t="inlineStr">
         <is>
-          <t>2020-02-26T00:00:00</t>
+          <t>2020-02-26</t>
         </is>
       </c>
       <c r="F375" t="inlineStr"/>
@@ -10147,7 +10031,7 @@
       </c>
       <c r="E378" t="inlineStr">
         <is>
-          <t>2020-02-27T00:00:00</t>
+          <t>2020-02-27</t>
         </is>
       </c>
       <c r="F378" t="inlineStr"/>
@@ -10197,7 +10081,7 @@
       </c>
       <c r="E380" t="inlineStr">
         <is>
-          <t>2020-02-29T00:00:00</t>
+          <t>2020-02-29</t>
         </is>
       </c>
       <c r="F380" t="inlineStr"/>
@@ -10247,7 +10131,7 @@
       </c>
       <c r="E382" t="inlineStr">
         <is>
-          <t>2020-03-01T00:00:00</t>
+          <t>2020-03-01</t>
         </is>
       </c>
       <c r="F382" t="inlineStr"/>
@@ -10297,7 +10181,7 @@
       </c>
       <c r="E384" t="inlineStr">
         <is>
-          <t>2020-03-02T00:00:00</t>
+          <t>2020-03-02</t>
         </is>
       </c>
       <c r="F384" t="inlineStr"/>
@@ -10425,7 +10309,7 @@
       </c>
       <c r="E389" t="inlineStr">
         <is>
-          <t>2020-03-04T00:00:00</t>
+          <t>2020-03-04</t>
         </is>
       </c>
       <c r="F389" t="inlineStr"/>
@@ -10569,7 +10453,7 @@
       </c>
       <c r="E394" t="inlineStr">
         <is>
-          <t>2020-03-05T00:00:00</t>
+          <t>2020-03-05</t>
         </is>
       </c>
       <c r="F394" t="inlineStr"/>
@@ -10663,7 +10547,7 @@
       </c>
       <c r="E397" t="inlineStr">
         <is>
-          <t>2020-03-06T00:00:00</t>
+          <t>2020-03-06</t>
         </is>
       </c>
       <c r="F397" t="inlineStr"/>
@@ -10747,7 +10631,7 @@
       </c>
       <c r="E400" t="inlineStr">
         <is>
-          <t>2020-03-07T00:00:00</t>
+          <t>2020-03-07</t>
         </is>
       </c>
       <c r="F400" t="inlineStr"/>
@@ -10801,7 +10685,7 @@
       </c>
       <c r="E402" t="inlineStr">
         <is>
-          <t>2020-03-08T00:00:00</t>
+          <t>2020-03-08</t>
         </is>
       </c>
       <c r="F402" t="inlineStr"/>
@@ -10855,7 +10739,7 @@
       </c>
       <c r="E404" t="inlineStr">
         <is>
-          <t>2020-03-10T00:00:00</t>
+          <t>2020-03-10</t>
         </is>
       </c>
       <c r="F404" t="inlineStr"/>
@@ -10931,7 +10815,7 @@
       </c>
       <c r="E407" t="inlineStr">
         <is>
-          <t>2020-03-11T00:00:00</t>
+          <t>2020-03-11</t>
         </is>
       </c>
       <c r="F407" t="inlineStr"/>
@@ -11033,7 +10917,7 @@
       </c>
       <c r="E411" t="inlineStr">
         <is>
-          <t>2020-03-13T00:00:00</t>
+          <t>2020-03-13</t>
         </is>
       </c>
       <c r="F411" t="inlineStr"/>
@@ -11087,7 +10971,7 @@
       </c>
       <c r="E413" t="inlineStr">
         <is>
-          <t>2020-03-14T00:00:00</t>
+          <t>2020-03-14</t>
         </is>
       </c>
       <c r="F413" t="inlineStr"/>
@@ -11201,7 +11085,7 @@
       </c>
       <c r="E417" t="inlineStr">
         <is>
-          <t>2020-03-15T00:00:00</t>
+          <t>2020-03-15</t>
         </is>
       </c>
       <c r="F417" t="inlineStr"/>
@@ -11315,7 +11199,7 @@
       </c>
       <c r="E421" t="inlineStr">
         <is>
-          <t>2020-03-16T00:00:00</t>
+          <t>2020-03-16</t>
         </is>
       </c>
       <c r="F421" t="inlineStr"/>
@@ -11385,7 +11269,7 @@
       </c>
       <c r="E424" t="inlineStr">
         <is>
-          <t>2020-03-17T00:00:00</t>
+          <t>2020-03-17</t>
         </is>
       </c>
       <c r="F424" t="inlineStr"/>
@@ -11485,7 +11369,7 @@
       </c>
       <c r="E428" t="inlineStr">
         <is>
-          <t>2020-03-18T00:00:00</t>
+          <t>2020-03-18</t>
         </is>
       </c>
       <c r="F428" t="inlineStr"/>
@@ -11539,7 +11423,7 @@
       </c>
       <c r="E430" t="inlineStr">
         <is>
-          <t>2020-03-20T00:00:00</t>
+          <t>2020-03-20</t>
         </is>
       </c>
       <c r="F430" t="inlineStr"/>
@@ -11589,7 +11473,7 @@
       </c>
       <c r="E432" t="inlineStr">
         <is>
-          <t>2020-03-22T00:00:00</t>
+          <t>2020-03-22</t>
         </is>
       </c>
       <c r="F432" t="inlineStr"/>
@@ -11639,7 +11523,7 @@
       </c>
       <c r="E434" t="inlineStr">
         <is>
-          <t>2020-03-23T00:00:00</t>
+          <t>2020-03-23</t>
         </is>
       </c>
       <c r="F434" t="inlineStr"/>
@@ -11715,7 +11599,7 @@
       </c>
       <c r="E437" t="inlineStr">
         <is>
-          <t>2020-04-02T00:00:00</t>
+          <t>2020-04-02</t>
         </is>
       </c>
       <c r="F437" t="inlineStr"/>
@@ -11765,7 +11649,7 @@
       </c>
       <c r="E439" t="inlineStr">
         <is>
-          <t>2020-04-03T00:00:00</t>
+          <t>2020-04-03</t>
         </is>
       </c>
       <c r="F439" t="inlineStr"/>
@@ -11815,7 +11699,7 @@
       </c>
       <c r="E441" t="inlineStr">
         <is>
-          <t>2020-04-14T00:00:00</t>
+          <t>2020-04-14</t>
         </is>
       </c>
       <c r="F441" t="inlineStr"/>
@@ -11865,7 +11749,7 @@
       </c>
       <c r="E443" t="inlineStr">
         <is>
-          <t>2020-04-17T00:00:00</t>
+          <t>2020-04-17</t>
         </is>
       </c>
       <c r="F443" t="inlineStr"/>
@@ -11915,7 +11799,7 @@
       </c>
       <c r="E445" t="inlineStr">
         <is>
-          <t>2020-04-18T00:00:00</t>
+          <t>2020-04-18</t>
         </is>
       </c>
       <c r="F445" t="inlineStr"/>
@@ -11965,7 +11849,7 @@
       </c>
       <c r="E447" t="inlineStr">
         <is>
-          <t>2020-04-27T00:00:00</t>
+          <t>2020-04-27</t>
         </is>
       </c>
       <c r="F447" t="inlineStr"/>
@@ -12041,7 +11925,7 @@
       </c>
       <c r="E450" t="inlineStr">
         <is>
-          <t>2020-05-07T00:00:00</t>
+          <t>2020-05-07</t>
         </is>
       </c>
       <c r="F450" t="inlineStr"/>
@@ -12087,7 +11971,7 @@
       </c>
       <c r="E452" t="inlineStr">
         <is>
-          <t>2020-05-09T00:00:00</t>
+          <t>2020-05-09</t>
         </is>
       </c>
       <c r="F452" t="inlineStr"/>
@@ -12133,7 +12017,7 @@
       </c>
       <c r="E454" t="inlineStr">
         <is>
-          <t>2020-05-13T00:00:00</t>
+          <t>2020-05-13</t>
         </is>
       </c>
       <c r="F454" t="inlineStr"/>
@@ -12179,7 +12063,7 @@
       </c>
       <c r="E456" t="inlineStr">
         <is>
-          <t>2020-05-15T00:00:00</t>
+          <t>2020-05-15</t>
         </is>
       </c>
       <c r="F456" t="inlineStr"/>
@@ -12251,7 +12135,7 @@
       </c>
       <c r="E459" t="inlineStr">
         <is>
-          <t>2020-05-16T00:00:00</t>
+          <t>2020-05-16</t>
         </is>
       </c>
       <c r="F459" t="inlineStr"/>
@@ -12297,7 +12181,7 @@
       </c>
       <c r="E461" t="inlineStr">
         <is>
-          <t>2020-05-20T00:00:00</t>
+          <t>2020-05-20</t>
         </is>
       </c>
       <c r="F461" t="inlineStr"/>
@@ -12343,7 +12227,7 @@
       </c>
       <c r="E463" t="inlineStr">
         <is>
-          <t>2020-05-22T00:00:00</t>
+          <t>2020-05-22</t>
         </is>
       </c>
       <c r="F463" t="inlineStr"/>
@@ -12389,7 +12273,7 @@
       </c>
       <c r="E465" t="inlineStr">
         <is>
-          <t>2020-05-28T00:00:00</t>
+          <t>2020-05-28</t>
         </is>
       </c>
       <c r="F465" t="inlineStr"/>
@@ -12487,7 +12371,7 @@
       </c>
       <c r="E469" t="inlineStr">
         <is>
-          <t>2020-06-02T00:00:00</t>
+          <t>2020-06-02</t>
         </is>
       </c>
       <c r="F469" t="inlineStr"/>
@@ -12533,7 +12417,7 @@
       </c>
       <c r="E471" t="inlineStr">
         <is>
-          <t>2020-06-03T00:00:00</t>
+          <t>2020-06-03</t>
         </is>
       </c>
       <c r="F471" t="inlineStr"/>
@@ -12631,7 +12515,7 @@
       </c>
       <c r="E475" t="inlineStr">
         <is>
-          <t>2020-06-04T00:00:00</t>
+          <t>2020-06-04</t>
         </is>
       </c>
       <c r="F475" t="inlineStr"/>
@@ -12677,7 +12561,7 @@
       </c>
       <c r="E477" t="inlineStr">
         <is>
-          <t>2020-06-05T00:00:00</t>
+          <t>2020-06-05</t>
         </is>
       </c>
       <c r="F477" t="inlineStr"/>
@@ -12723,7 +12607,7 @@
       </c>
       <c r="E479" t="inlineStr">
         <is>
-          <t>2020-06-08T00:00:00</t>
+          <t>2020-06-08</t>
         </is>
       </c>
       <c r="F479" t="inlineStr"/>
@@ -12765,7 +12649,7 @@
       </c>
       <c r="E481" t="inlineStr">
         <is>
-          <t>2020-06-10T00:00:00</t>
+          <t>2020-06-10</t>
         </is>
       </c>
       <c r="F481" t="inlineStr"/>
@@ -12811,7 +12695,7 @@
       </c>
       <c r="E483" t="inlineStr">
         <is>
-          <t>2020-06-12T00:00:00</t>
+          <t>2020-06-12</t>
         </is>
       </c>
       <c r="F483" t="inlineStr"/>
@@ -12879,7 +12763,7 @@
       </c>
       <c r="E486" t="inlineStr">
         <is>
-          <t>2020-06-13T00:00:00</t>
+          <t>2020-06-13</t>
         </is>
       </c>
       <c r="F486" t="inlineStr"/>
@@ -12921,7 +12805,7 @@
       </c>
       <c r="E488" t="inlineStr">
         <is>
-          <t>2020-06-14T00:00:00</t>
+          <t>2020-06-14</t>
         </is>
       </c>
       <c r="F488" t="inlineStr"/>
@@ -12963,7 +12847,7 @@
       </c>
       <c r="E490" t="inlineStr">
         <is>
-          <t>2020-06-15T00:00:00</t>
+          <t>2020-06-15</t>
         </is>
       </c>
       <c r="F490" t="inlineStr"/>
@@ -13009,7 +12893,7 @@
       </c>
       <c r="E492" t="inlineStr">
         <is>
-          <t>2020-06-16T00:00:00</t>
+          <t>2020-06-16</t>
         </is>
       </c>
       <c r="F492" t="inlineStr"/>
@@ -13081,7 +12965,7 @@
       </c>
       <c r="E495" t="inlineStr">
         <is>
-          <t>2020-06-17T00:00:00</t>
+          <t>2020-06-17</t>
         </is>
       </c>
       <c r="F495" t="inlineStr"/>
@@ -13127,7 +13011,7 @@
       </c>
       <c r="E497" t="inlineStr">
         <is>
-          <t>2020-06-18T00:00:00</t>
+          <t>2020-06-18</t>
         </is>
       </c>
       <c r="F497" t="inlineStr"/>
@@ -13169,7 +13053,7 @@
       </c>
       <c r="E499" t="inlineStr">
         <is>
-          <t>2020-06-22T00:00:00</t>
+          <t>2020-06-22</t>
         </is>
       </c>
       <c r="F499" t="inlineStr"/>
@@ -13241,7 +13125,7 @@
       </c>
       <c r="E502" t="inlineStr">
         <is>
-          <t>2020-06-26T00:00:00</t>
+          <t>2020-06-26</t>
         </is>
       </c>
       <c r="F502" t="inlineStr"/>
@@ -13309,7 +13193,7 @@
       </c>
       <c r="E505" t="inlineStr">
         <is>
-          <t>2020-07-01T00:00:00</t>
+          <t>2020-07-01</t>
         </is>
       </c>
       <c r="F505" t="inlineStr"/>
@@ -13355,7 +13239,7 @@
       </c>
       <c r="E507" t="inlineStr">
         <is>
-          <t>2020-07-03T00:00:00</t>
+          <t>2020-07-03</t>
         </is>
       </c>
       <c r="F507" t="inlineStr"/>
@@ -13401,7 +13285,7 @@
       </c>
       <c r="E509" t="inlineStr">
         <is>
-          <t>2020-07-04T00:00:00</t>
+          <t>2020-07-04</t>
         </is>
       </c>
       <c r="F509" t="inlineStr"/>
@@ -13469,7 +13353,7 @@
       </c>
       <c r="E512" t="inlineStr">
         <is>
-          <t>2020-07-07T00:00:00</t>
+          <t>2020-07-07</t>
         </is>
       </c>
       <c r="F512" t="inlineStr"/>
@@ -13541,7 +13425,7 @@
       </c>
       <c r="E515" t="inlineStr">
         <is>
-          <t>2020-07-08T00:00:00</t>
+          <t>2020-07-08</t>
         </is>
       </c>
       <c r="F515" t="inlineStr"/>
@@ -13639,7 +13523,7 @@
       </c>
       <c r="E519" t="inlineStr">
         <is>
-          <t>2020-07-10T00:00:00</t>
+          <t>2020-07-10</t>
         </is>
       </c>
       <c r="F519" t="inlineStr"/>
@@ -13785,7 +13669,7 @@
       </c>
       <c r="E525" t="inlineStr">
         <is>
-          <t>2020-07-14T00:00:00</t>
+          <t>2020-07-14</t>
         </is>
       </c>
       <c r="F525" t="inlineStr"/>
@@ -13831,7 +13715,7 @@
       </c>
       <c r="E527" t="inlineStr">
         <is>
-          <t>2020-07-15T00:00:00</t>
+          <t>2020-07-15</t>
         </is>
       </c>
       <c r="F527" t="inlineStr"/>
@@ -13877,7 +13761,7 @@
       </c>
       <c r="E529" t="inlineStr">
         <is>
-          <t>2020-07-16T00:00:00</t>
+          <t>2020-07-16</t>
         </is>
       </c>
       <c r="F529" t="inlineStr"/>
@@ -13975,7 +13859,7 @@
       </c>
       <c r="E533" t="inlineStr">
         <is>
-          <t>2020-07-19T00:00:00</t>
+          <t>2020-07-19</t>
         </is>
       </c>
       <c r="F533" t="inlineStr"/>
@@ -14073,7 +13957,7 @@
       </c>
       <c r="E537" t="inlineStr">
         <is>
-          <t>2020-07-20T00:00:00</t>
+          <t>2020-07-20</t>
         </is>
       </c>
       <c r="F537" t="inlineStr"/>
@@ -14167,7 +14051,7 @@
       </c>
       <c r="E541" t="inlineStr">
         <is>
-          <t>2020-07-21T00:00:00</t>
+          <t>2020-07-21</t>
         </is>
       </c>
       <c r="F541" t="inlineStr"/>
@@ -14235,7 +14119,7 @@
       </c>
       <c r="E544" t="inlineStr">
         <is>
-          <t>2020-07-22T00:00:00</t>
+          <t>2020-07-22</t>
         </is>
       </c>
       <c r="F544" t="inlineStr"/>
@@ -14281,7 +14165,7 @@
       </c>
       <c r="E546" t="inlineStr">
         <is>
-          <t>2020-07-24T00:00:00</t>
+          <t>2020-07-24</t>
         </is>
       </c>
       <c r="F546" t="inlineStr"/>
@@ -14323,7 +14207,7 @@
       </c>
       <c r="E548" t="inlineStr">
         <is>
-          <t>2020-07-25T00:00:00</t>
+          <t>2020-07-25</t>
         </is>
       </c>
       <c r="F548" t="inlineStr"/>
@@ -14369,7 +14253,7 @@
       </c>
       <c r="E550" t="inlineStr">
         <is>
-          <t>2020-07-28T00:00:00</t>
+          <t>2020-07-28</t>
         </is>
       </c>
       <c r="F550" t="inlineStr"/>
@@ -14415,7 +14299,7 @@
       </c>
       <c r="E552" t="inlineStr">
         <is>
-          <t>2020-07-29T00:00:00</t>
+          <t>2020-07-29</t>
         </is>
       </c>
       <c r="F552" t="inlineStr"/>
@@ -14595,7 +14479,7 @@
       </c>
       <c r="E559" t="inlineStr">
         <is>
-          <t>2020-07-30T00:00:00</t>
+          <t>2020-07-30</t>
         </is>
       </c>
       <c r="F559" t="inlineStr"/>
@@ -14693,7 +14577,7 @@
       </c>
       <c r="E563" t="inlineStr">
         <is>
-          <t>2020-08-03T00:00:00</t>
+          <t>2020-08-03</t>
         </is>
       </c>
       <c r="F563" t="inlineStr"/>
@@ -14787,7 +14671,7 @@
       </c>
       <c r="E567" t="inlineStr">
         <is>
-          <t>2020-08-07T00:00:00</t>
+          <t>2020-08-07</t>
         </is>
       </c>
       <c r="F567" t="inlineStr"/>
@@ -14833,7 +14717,7 @@
       </c>
       <c r="E569" t="inlineStr">
         <is>
-          <t>2020-08-08T00:00:00</t>
+          <t>2020-08-08</t>
         </is>
       </c>
       <c r="F569" t="inlineStr"/>
@@ -14879,7 +14763,7 @@
       </c>
       <c r="E571" t="inlineStr">
         <is>
-          <t>2020-08-09T00:00:00</t>
+          <t>2020-08-09</t>
         </is>
       </c>
       <c r="F571" t="inlineStr"/>
@@ -14925,7 +14809,7 @@
       </c>
       <c r="E573" t="inlineStr">
         <is>
-          <t>2020-08-11T00:00:00</t>
+          <t>2020-08-11</t>
         </is>
       </c>
       <c r="F573" t="inlineStr"/>
@@ -14971,7 +14855,7 @@
       </c>
       <c r="E575" t="inlineStr">
         <is>
-          <t>2020-08-14T00:00:00</t>
+          <t>2020-08-14</t>
         </is>
       </c>
       <c r="F575" t="inlineStr"/>
@@ -15017,7 +14901,7 @@
       </c>
       <c r="E577" t="inlineStr">
         <is>
-          <t>2020-08-16T00:00:00</t>
+          <t>2020-08-16</t>
         </is>
       </c>
       <c r="F577" t="inlineStr"/>
@@ -15089,7 +14973,7 @@
       </c>
       <c r="E580" t="inlineStr">
         <is>
-          <t>2020-08-18T00:00:00</t>
+          <t>2020-08-18</t>
         </is>
       </c>
       <c r="F580" t="inlineStr"/>
@@ -15135,7 +15019,7 @@
       </c>
       <c r="E582" t="inlineStr">
         <is>
-          <t>2020-08-20T00:00:00</t>
+          <t>2020-08-20</t>
         </is>
       </c>
       <c r="F582" t="inlineStr"/>
@@ -15183,7 +15067,7 @@
       </c>
       <c r="E584" t="inlineStr">
         <is>
-          <t>2020-08-22T00:00:00</t>
+          <t>2020-08-22</t>
         </is>
       </c>
       <c r="F584" t="inlineStr"/>
@@ -15241,7 +15125,7 @@
       </c>
       <c r="E587" t="inlineStr">
         <is>
-          <t>2020-08-25T00:00:00</t>
+          <t>2020-08-25</t>
         </is>
       </c>
       <c r="F587" t="inlineStr"/>
@@ -15289,7 +15173,7 @@
       </c>
       <c r="E589" t="inlineStr">
         <is>
-          <t>2020-08-26T00:00:00</t>
+          <t>2020-08-26</t>
         </is>
       </c>
       <c r="F589" t="inlineStr"/>

</xml_diff>